<commit_message>
Actualizados los archivos y agregados ABCDE . pdf
</commit_message>
<xml_diff>
--- a/Proyecto final/Documentacion Final Optical Marketing/Informes e Investigaciones/KinectsSDKDAR.xlsx
+++ b/Proyecto final/Documentacion Final Optical Marketing/Informes e Investigaciones/KinectsSDKDAR.xlsx
@@ -512,20 +512,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,6 +531,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,97 +847,99 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C15"/>
+      <selection sqref="A1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="32" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="39.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A2" s="12"/>
+      <c r="A2" s="8"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:12" s="15" customFormat="1" ht="60" customHeight="1" thickBot="1">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -963,7 +977,7 @@
       <c r="K4" s="1">
         <v>40</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="6">
         <f>SUM(B4:K4)</f>
         <v>745</v>
       </c>
@@ -1002,7 +1016,7 @@
       <c r="K5" s="1">
         <v>65</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="6">
         <f t="shared" ref="L5:L6" si="0">SUM(B5:K5)</f>
         <v>640</v>
       </c>
@@ -1041,62 +1055,90 @@
       <c r="K6" s="1">
         <v>80</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
         <v>705</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="14"/>
+      <c r="B16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A9:C15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A9:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>